<commit_message>
broken commit - fix at work
</commit_message>
<xml_diff>
--- a/crunch/src/test/resources/DataTest.xlsx
+++ b/crunch/src/test/resources/DataTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26160" yWindow="1980" windowWidth="21520" windowHeight="18380" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="26640" yWindow="760" windowWidth="26740" windowHeight="21880" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ZScore10Day" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="17">
   <si>
     <t>Close</t>
   </si>
@@ -63,12 +63,24 @@
   <si>
     <t>AvgVolPost30Days</t>
   </si>
+  <si>
+    <t>TotPricePre30Days</t>
+  </si>
+  <si>
+    <t>TotVolPre30Days</t>
+  </si>
+  <si>
+    <t>AvgPricePre30Days</t>
+  </si>
+  <si>
+    <t>AvgVolPre30Day</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,13 +104,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,17 +134,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9745,21 +9780,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4880"/>
+  <dimension ref="A1:L4880"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9784,8 +9824,20 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>19850102</v>
       </c>
@@ -9796,7 +9848,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>19850103</v>
       </c>
@@ -9807,7 +9859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>19850104</v>
       </c>
@@ -9818,7 +9870,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>19850107</v>
       </c>
@@ -9829,7 +9881,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>19850108</v>
       </c>
@@ -9840,7 +9892,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>19850110</v>
       </c>
@@ -9851,7 +9903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>19850111</v>
       </c>
@@ -9862,7 +9914,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>19850115</v>
       </c>
@@ -9873,7 +9925,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>19850117</v>
       </c>
@@ -9884,7 +9936,7 @@
         <v>5550</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>19850118</v>
       </c>
@@ -9895,7 +9947,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>19850121</v>
       </c>
@@ -9906,7 +9958,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>19850122</v>
       </c>
@@ -9917,7 +9969,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>19850123</v>
       </c>
@@ -9928,7 +9980,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>19850124</v>
       </c>
@@ -9939,7 +9991,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>19850125</v>
       </c>
@@ -9950,7 +10002,7 @@
         <v>5050</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>19850128</v>
       </c>
@@ -9961,7 +10013,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>19850129</v>
       </c>
@@ -9972,7 +10024,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>19850130</v>
       </c>
@@ -9983,7 +10035,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>19850131</v>
       </c>
@@ -9994,7 +10046,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>19850201</v>
       </c>
@@ -10016,8 +10068,24 @@
       <c r="H21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <f>SUM(B21:B37)</f>
+        <v>586</v>
+      </c>
+      <c r="J21">
+        <f>SUM(C21:C37)</f>
+        <v>8900</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE(B21:B37)</f>
+        <v>34.470588235294116</v>
+      </c>
+      <c r="L21">
+        <f>AVERAGE(C21:C37)</f>
+        <v>523.52941176470586</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>19850204</v>
       </c>
@@ -10028,7 +10096,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>19850205</v>
       </c>
@@ -10039,7 +10107,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>19850207</v>
       </c>
@@ -10050,7 +10118,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>19850208</v>
       </c>
@@ -10061,7 +10129,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>19850211</v>
       </c>
@@ -10072,7 +10140,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>19850213</v>
       </c>
@@ -10083,7 +10151,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>19850215</v>
       </c>
@@ -10094,7 +10162,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>19850219</v>
       </c>
@@ -10105,7 +10173,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>19850221</v>
       </c>
@@ -10116,7 +10184,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>19850222</v>
       </c>
@@ -10127,7 +10195,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>19850225</v>
       </c>
@@ -10138,7 +10206,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>19850226</v>
       </c>
@@ -10149,7 +10217,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>19850227</v>
       </c>
@@ -10160,7 +10228,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>19850228</v>
       </c>
@@ -10171,7 +10239,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>19850301</v>
       </c>
@@ -10182,7 +10250,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>19850308</v>
       </c>
@@ -10208,8 +10276,20 @@
         <f>AVERAGE(C21:C37)</f>
         <v>523.52941176470586</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>19850315</v>
       </c>
@@ -10220,7 +10300,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>19850318</v>
       </c>
@@ -10231,7 +10311,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>19850319</v>
       </c>
@@ -10242,7 +10322,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>19850320</v>
       </c>
@@ -10253,30 +10333,30 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42">
+    <row r="42" spans="1:12" s="1" customFormat="1">
+      <c r="A42" s="1">
         <v>19850322</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>31.5</v>
       </c>
-      <c r="C42">
-        <v>100</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="C42" s="1">
+        <v>100</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>19850326</v>
       </c>
@@ -10286,8 +10366,24 @@
       <c r="C43">
         <v>200</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" s="1">
+        <f>SUM(B43:B53)</f>
+        <v>356.125</v>
+      </c>
+      <c r="J43" s="1">
+        <f>SUM(C43:C53)</f>
+        <v>37450</v>
+      </c>
+      <c r="K43" s="1">
+        <f>AVERAGE(B43:B53)</f>
+        <v>32.375</v>
+      </c>
+      <c r="L43" s="1">
+        <f>AVERAGE(C43:C53)</f>
+        <v>3404.5454545454545</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>19850327</v>
       </c>
@@ -10298,7 +10394,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>19850329</v>
       </c>
@@ -10309,7 +10405,7 @@
         <v>31600</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>19850401</v>
       </c>
@@ -10320,7 +10416,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>19850402</v>
       </c>
@@ -10331,7 +10427,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>19850415</v>
       </c>
@@ -10342,7 +10438,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>19850416</v>
       </c>
@@ -10353,7 +10449,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>19850417</v>
       </c>
@@ -10364,7 +10460,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>19850418</v>
       </c>
@@ -10375,34 +10471,46 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
-      <c r="A52">
+    <row r="52" spans="1:12" s="1" customFormat="1">
+      <c r="A52" s="1">
         <v>19850422</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>33</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>350</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="1">
         <f>SUM(B42:B52)</f>
         <v>354.75</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <f>SUM(C42:C52)</f>
         <v>37450</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="1">
         <f>AVERAGE(B42:B52)</f>
         <v>32.25</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="1">
         <f>AVERAGE(C42:C52)</f>
         <v>3404.5454545454545</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>19850423</v>
       </c>
@@ -10413,7 +10521,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>19850424</v>
       </c>
@@ -10424,7 +10532,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>19850425</v>
       </c>
@@ -10446,8 +10554,24 @@
       <c r="H55" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55">
+        <f>SUM(B55:B70)</f>
+        <v>540.25</v>
+      </c>
+      <c r="J55">
+        <f>SUM(C55:C70)</f>
+        <v>10300</v>
+      </c>
+      <c r="K55">
+        <f>AVERAGE(B55:B70)</f>
+        <v>33.765625</v>
+      </c>
+      <c r="L55">
+        <f>AVERAGE(C55:C70)</f>
+        <v>643.75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>19850426</v>
       </c>
@@ -10458,7 +10582,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>19850430</v>
       </c>
@@ -10469,7 +10593,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:12">
       <c r="A58">
         <v>19850501</v>
       </c>
@@ -10480,7 +10604,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:12">
       <c r="A59">
         <v>19850502</v>
       </c>
@@ -10491,7 +10615,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:12">
       <c r="A60">
         <v>19850503</v>
       </c>
@@ -10502,7 +10626,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:12">
       <c r="A61">
         <v>19850507</v>
       </c>
@@ -10513,7 +10637,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:12">
       <c r="A62">
         <v>19850508</v>
       </c>
@@ -10524,7 +10648,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:12">
       <c r="A63">
         <v>19850509</v>
       </c>
@@ -10535,7 +10659,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:12">
       <c r="A64">
         <v>19850513</v>
       </c>
@@ -10546,7 +10670,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:12">
       <c r="A65">
         <v>19850520</v>
       </c>
@@ -10557,7 +10681,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:12">
       <c r="A66">
         <v>19850521</v>
       </c>
@@ -10568,7 +10692,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:12">
       <c r="A67">
         <v>19850522</v>
       </c>
@@ -10579,7 +10703,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:12">
       <c r="A68">
         <v>19850523</v>
       </c>
@@ -10590,7 +10714,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:12">
       <c r="A69">
         <v>19850524</v>
       </c>
@@ -10601,7 +10725,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:12">
       <c r="A70">
         <v>19850529</v>
       </c>
@@ -10627,8 +10751,20 @@
         <f>AVERAGE(C55:C70)</f>
         <v>643.75</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70" t="s">
+        <v>7</v>
+      </c>
+      <c r="J70" t="s">
+        <v>7</v>
+      </c>
+      <c r="K70" t="s">
+        <v>7</v>
+      </c>
+      <c r="L70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71">
         <v>19850530</v>
       </c>
@@ -10639,7 +10775,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:12">
       <c r="A72">
         <v>19850531</v>
       </c>
@@ -10650,7 +10786,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:12">
       <c r="A73">
         <v>19850603</v>
       </c>
@@ -10661,7 +10797,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:12">
       <c r="A74">
         <v>19850605</v>
       </c>
@@ -10672,7 +10808,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:12">
       <c r="A75">
         <v>19850606</v>
       </c>
@@ -10683,7 +10819,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:12">
       <c r="A76">
         <v>19850607</v>
       </c>
@@ -10694,7 +10830,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:12">
       <c r="A77">
         <v>19850611</v>
       </c>
@@ -10705,7 +10841,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:12">
       <c r="A78">
         <v>19850613</v>
       </c>
@@ -10716,7 +10852,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:12">
       <c r="A79">
         <v>19850614</v>
       </c>
@@ -10727,7 +10863,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:12">
       <c r="A80">
         <v>19850617</v>
       </c>
@@ -10738,7 +10874,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:12">
       <c r="A81">
         <v>19850618</v>
       </c>
@@ -10749,7 +10885,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:12">
       <c r="A82">
         <v>19850619</v>
       </c>
@@ -10760,7 +10896,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:12">
       <c r="A83">
         <v>19850624</v>
       </c>
@@ -10771,7 +10907,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:12">
       <c r="A84">
         <v>19850625</v>
       </c>
@@ -10782,7 +10918,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:12">
       <c r="A85">
         <v>19850626</v>
       </c>
@@ -10793,7 +10929,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:12">
       <c r="A86">
         <v>19850628</v>
       </c>
@@ -10804,7 +10940,7 @@
         <v>31900</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:12">
       <c r="A87">
         <v>19850701</v>
       </c>
@@ -10815,7 +10951,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:12">
       <c r="A88">
         <v>19850702</v>
       </c>
@@ -10826,7 +10962,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:12">
       <c r="A89">
         <v>19850703</v>
       </c>
@@ -10837,7 +10973,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:12">
       <c r="A90">
         <v>19850705</v>
       </c>
@@ -10848,7 +10984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:12">
       <c r="A91">
         <v>19850708</v>
       </c>
@@ -10859,7 +10995,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:12">
       <c r="A92">
         <v>19850709</v>
       </c>
@@ -10870,7 +11006,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:12">
       <c r="A93">
         <v>19850710</v>
       </c>
@@ -10892,8 +11028,24 @@
       <c r="H93" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93">
+        <f>SUM(B93:B108)</f>
+        <v>553.25</v>
+      </c>
+      <c r="J93">
+        <f>SUM(C93:C108)</f>
+        <v>26050</v>
+      </c>
+      <c r="K93">
+        <f>AVERAGE(B93:B108)</f>
+        <v>34.578125</v>
+      </c>
+      <c r="L93">
+        <f>AVERAGE(C93:C108)</f>
+        <v>1628.125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94">
         <v>19850711</v>
       </c>
@@ -10904,7 +11056,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:12">
       <c r="A95">
         <v>19850712</v>
       </c>
@@ -10915,7 +11067,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:12">
       <c r="A96">
         <v>19850715</v>
       </c>
@@ -10926,7 +11078,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:12">
       <c r="A97">
         <v>19850717</v>
       </c>
@@ -10937,7 +11089,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:12">
       <c r="A98">
         <v>19850719</v>
       </c>
@@ -10948,7 +11100,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:12">
       <c r="A99">
         <v>19850722</v>
       </c>
@@ -10959,7 +11111,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:12">
       <c r="A100">
         <v>19850723</v>
       </c>
@@ -10970,7 +11122,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:12">
       <c r="A101">
         <v>19850724</v>
       </c>
@@ -10981,7 +11133,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:12">
       <c r="A102">
         <v>19850725</v>
       </c>
@@ -10992,7 +11144,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:12">
       <c r="A103">
         <v>19850726</v>
       </c>
@@ -11003,7 +11155,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:12">
       <c r="A104">
         <v>19850729</v>
       </c>
@@ -11014,7 +11166,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:12">
       <c r="A105">
         <v>19850802</v>
       </c>
@@ -11025,7 +11177,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:12">
       <c r="A106">
         <v>19850806</v>
       </c>
@@ -11036,7 +11188,7 @@
         <v>13750</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:12">
       <c r="A107">
         <v>19850808</v>
       </c>
@@ -11047,7 +11199,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:12">
       <c r="A108">
         <v>19850809</v>
       </c>
@@ -11073,8 +11225,20 @@
         <f>AVERAGE(C93:C108)</f>
         <v>1628.125</v>
       </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="I108" t="s">
+        <v>7</v>
+      </c>
+      <c r="J108" t="s">
+        <v>7</v>
+      </c>
+      <c r="K108" t="s">
+        <v>7</v>
+      </c>
+      <c r="L108" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109">
         <v>19850812</v>
       </c>
@@ -11085,7 +11249,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:12">
       <c r="A110">
         <v>19850813</v>
       </c>
@@ -11096,7 +11260,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:12">
       <c r="A111">
         <v>19850814</v>
       </c>
@@ -11107,7 +11271,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:12">
       <c r="A112">
         <v>19850815</v>
       </c>
@@ -11118,7 +11282,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:12">
       <c r="A113">
         <v>19850816</v>
       </c>
@@ -11129,7 +11293,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:12">
       <c r="A114">
         <v>19850819</v>
       </c>
@@ -11140,7 +11304,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:12">
       <c r="A115">
         <v>19850820</v>
       </c>
@@ -11151,7 +11315,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:12">
       <c r="A116">
         <v>19850821</v>
       </c>
@@ -11162,7 +11326,7 @@
         <v>9950</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:12">
       <c r="A117">
         <v>19850823</v>
       </c>
@@ -11173,7 +11337,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:12">
       <c r="A118">
         <v>19850826</v>
       </c>
@@ -11184,7 +11348,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:12">
       <c r="A119">
         <v>19850828</v>
       </c>
@@ -11195,7 +11359,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:12">
       <c r="A120">
         <v>19850830</v>
       </c>
@@ -11206,7 +11370,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:12">
       <c r="A121">
         <v>19850903</v>
       </c>
@@ -11217,7 +11381,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:12">
       <c r="A122">
         <v>19850904</v>
       </c>
@@ -11228,7 +11392,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:12">
       <c r="A123">
         <v>19850906</v>
       </c>
@@ -11239,7 +11403,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:12">
       <c r="A124">
         <v>19850909</v>
       </c>
@@ -11250,7 +11414,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:12">
       <c r="A125">
         <v>19850910</v>
       </c>
@@ -11272,8 +11436,24 @@
       <c r="H125" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="I125">
+        <f>SUM(B125:B143)</f>
+        <v>639.25</v>
+      </c>
+      <c r="J125">
+        <f>SUM(C125:C143)</f>
+        <v>19050</v>
+      </c>
+      <c r="K125">
+        <f>AVERAGE(B125:B143)</f>
+        <v>33.64473684210526</v>
+      </c>
+      <c r="L125">
+        <f>AVERAGE(C125:C143)</f>
+        <v>1002.6315789473684</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126">
         <v>19850911</v>
       </c>
@@ -11284,7 +11464,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:12">
       <c r="A127">
         <v>19850913</v>
       </c>
@@ -11295,7 +11475,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:12">
       <c r="A128">
         <v>19850916</v>
       </c>
@@ -11306,7 +11486,7 @@
         <v>10650</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:12">
       <c r="A129">
         <v>19850918</v>
       </c>
@@ -11317,7 +11497,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:12">
       <c r="A130">
         <v>19850920</v>
       </c>
@@ -11328,7 +11508,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:12">
       <c r="A131">
         <v>19850923</v>
       </c>
@@ -11339,7 +11519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:12">
       <c r="A132">
         <v>19850924</v>
       </c>
@@ -11350,7 +11530,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:12">
       <c r="A133">
         <v>19850925</v>
       </c>
@@ -11361,7 +11541,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:12">
       <c r="A134">
         <v>19850926</v>
       </c>
@@ -11372,7 +11552,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:12">
       <c r="A135">
         <v>19850930</v>
       </c>
@@ -11383,7 +11563,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:12">
       <c r="A136">
         <v>19851001</v>
       </c>
@@ -11394,7 +11574,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:12">
       <c r="A137">
         <v>19851002</v>
       </c>
@@ -11405,7 +11585,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:12">
       <c r="A138">
         <v>19851003</v>
       </c>
@@ -11416,7 +11596,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:12">
       <c r="A139">
         <v>19851004</v>
       </c>
@@ -11427,7 +11607,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:12">
       <c r="A140">
         <v>19851007</v>
       </c>
@@ -11438,7 +11618,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:12">
       <c r="A141">
         <v>19851008</v>
       </c>
@@ -11449,7 +11629,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:12">
       <c r="A142">
         <v>19851009</v>
       </c>
@@ -11460,7 +11640,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:12">
       <c r="A143">
         <v>19851010</v>
       </c>
@@ -11486,8 +11666,20 @@
         <f>AVERAGE(C125:C143)</f>
         <v>1002.6315789473684</v>
       </c>
-    </row>
-    <row r="144" spans="1:8">
+      <c r="I143" t="s">
+        <v>7</v>
+      </c>
+      <c r="J143" t="s">
+        <v>7</v>
+      </c>
+      <c r="K143" t="s">
+        <v>7</v>
+      </c>
+      <c r="L143" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
       <c r="A144">
         <v>19851014</v>
       </c>
@@ -11850,7 +12042,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:12">
       <c r="A177">
         <v>19851204</v>
       </c>
@@ -11861,7 +12053,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:12">
       <c r="A178">
         <v>19851205</v>
       </c>
@@ -11872,7 +12064,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:12">
       <c r="A179">
         <v>19851206</v>
       </c>
@@ -11883,7 +12075,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:12">
       <c r="A180">
         <v>19851209</v>
       </c>
@@ -11894,7 +12086,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:12">
       <c r="A181">
         <v>19851210</v>
       </c>
@@ -11905,7 +12097,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:12">
       <c r="A182">
         <v>19851211</v>
       </c>
@@ -11916,7 +12108,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:12">
       <c r="A183">
         <v>19851212</v>
       </c>
@@ -11927,7 +12119,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:12">
       <c r="A184">
         <v>19851213</v>
       </c>
@@ -11938,7 +12130,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:12">
       <c r="A185">
         <v>19851217</v>
       </c>
@@ -11960,8 +12152,24 @@
       <c r="H185" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="186" spans="1:8">
+      <c r="I185">
+        <f>SUM(B185:B203)</f>
+        <v>669.375</v>
+      </c>
+      <c r="J185">
+        <f>SUM(C185:C203)</f>
+        <v>39750</v>
+      </c>
+      <c r="K185">
+        <f>AVERAGE(B185:B203)</f>
+        <v>35.23026315789474</v>
+      </c>
+      <c r="L185">
+        <f>AVERAGE(C185:C203)</f>
+        <v>2092.1052631578946</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12">
       <c r="A186">
         <v>19851218</v>
       </c>
@@ -11972,7 +12180,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:12">
       <c r="A187">
         <v>19851219</v>
       </c>
@@ -11983,7 +12191,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:12">
       <c r="A188">
         <v>19851220</v>
       </c>
@@ -11994,7 +12202,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:12">
       <c r="A189">
         <v>19851223</v>
       </c>
@@ -12005,7 +12213,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:12">
       <c r="A190">
         <v>19851224</v>
       </c>
@@ -12016,7 +12224,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:12">
       <c r="A191">
         <v>19851227</v>
       </c>
@@ -12027,7 +12235,7 @@
         <v>18500</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:12">
       <c r="A192">
         <v>19851230</v>
       </c>
@@ -12038,7 +12246,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:12">
       <c r="A193">
         <v>19851231</v>
       </c>
@@ -12052,7 +12260,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:12">
       <c r="A194">
         <v>19860102</v>
       </c>
@@ -12063,7 +12271,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:12">
       <c r="A195">
         <v>19860103</v>
       </c>
@@ -12074,7 +12282,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:12">
       <c r="A196">
         <v>19860106</v>
       </c>
@@ -12085,7 +12293,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:12">
       <c r="A197">
         <v>19860107</v>
       </c>
@@ -12096,7 +12304,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:12">
       <c r="A198">
         <v>19860108</v>
       </c>
@@ -12107,7 +12315,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:12">
       <c r="A199">
         <v>19860109</v>
       </c>
@@ -12118,7 +12326,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:12">
       <c r="A200">
         <v>19860110</v>
       </c>
@@ -12129,7 +12337,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:12">
       <c r="A201">
         <v>19860113</v>
       </c>
@@ -12140,7 +12348,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:12">
       <c r="A202">
         <v>19860115</v>
       </c>
@@ -12151,7 +12359,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:12">
       <c r="A203">
         <v>19860116</v>
       </c>
@@ -12177,8 +12385,20 @@
         <f>AVERAGE(C185:C203)</f>
         <v>2092.1052631578946</v>
       </c>
-    </row>
-    <row r="204" spans="1:8">
+      <c r="I203" t="s">
+        <v>7</v>
+      </c>
+      <c r="J203" t="s">
+        <v>7</v>
+      </c>
+      <c r="K203" t="s">
+        <v>7</v>
+      </c>
+      <c r="L203" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12">
       <c r="A204">
         <v>19860117</v>
       </c>
@@ -12189,7 +12409,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:12">
       <c r="A205">
         <v>19860121</v>
       </c>
@@ -12200,7 +12420,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:12">
       <c r="A206">
         <v>19860122</v>
       </c>
@@ -12211,7 +12431,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:12">
       <c r="A207">
         <v>19860123</v>
       </c>
@@ -12222,7 +12442,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:12">
       <c r="A208">
         <v>19860124</v>
       </c>
@@ -13289,7 +13509,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="305" spans="1:8">
+    <row r="305" spans="1:12">
       <c r="A305">
         <v>19860623</v>
       </c>
@@ -13300,7 +13520,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:12">
       <c r="A306">
         <v>19860624</v>
       </c>
@@ -13311,7 +13531,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="307" spans="1:8">
+    <row r="307" spans="1:12">
       <c r="A307">
         <v>19860625</v>
       </c>
@@ -13322,7 +13542,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="308" spans="1:8">
+    <row r="308" spans="1:12">
       <c r="A308">
         <v>19860626</v>
       </c>
@@ -13333,7 +13553,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:12">
       <c r="A309">
         <v>19860627</v>
       </c>
@@ -13344,7 +13564,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:12">
       <c r="A310">
         <v>19860630</v>
       </c>
@@ -13355,7 +13575,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="311" spans="1:8">
+    <row r="311" spans="1:12">
       <c r="A311">
         <v>19860701</v>
       </c>
@@ -13366,7 +13586,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:12">
       <c r="A312">
         <v>19860702</v>
       </c>
@@ -13377,7 +13597,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="313" spans="1:8">
+    <row r="313" spans="1:12">
       <c r="A313">
         <v>19860703</v>
       </c>
@@ -13388,7 +13608,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="314" spans="1:8">
+    <row r="314" spans="1:12">
       <c r="A314">
         <v>19860707</v>
       </c>
@@ -13410,8 +13630,24 @@
       <c r="H314" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="315" spans="1:8">
+      <c r="I314">
+        <f>SUM(B314:B332)</f>
+        <v>782.375</v>
+      </c>
+      <c r="J314">
+        <f>SUM(C314:C332)</f>
+        <v>12550</v>
+      </c>
+      <c r="K314">
+        <f>AVERAGE(B314:B332)</f>
+        <v>41.17763157894737</v>
+      </c>
+      <c r="L314">
+        <f>AVERAGE(C314:C332)</f>
+        <v>660.52631578947364</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12">
       <c r="A315">
         <v>19860708</v>
       </c>
@@ -13422,7 +13658,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:12">
       <c r="A316">
         <v>19860709</v>
       </c>
@@ -13433,7 +13669,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:12">
       <c r="A317">
         <v>19860711</v>
       </c>
@@ -13444,7 +13680,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="318" spans="1:8">
+    <row r="318" spans="1:12">
       <c r="A318">
         <v>19860714</v>
       </c>
@@ -13455,7 +13691,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="319" spans="1:8">
+    <row r="319" spans="1:12">
       <c r="A319">
         <v>19860715</v>
       </c>
@@ -13466,7 +13702,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:12">
       <c r="A320">
         <v>19860716</v>
       </c>
@@ -13477,7 +13713,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="321" spans="1:8">
+    <row r="321" spans="1:12">
       <c r="A321">
         <v>19860717</v>
       </c>
@@ -13488,7 +13724,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="322" spans="1:8">
+    <row r="322" spans="1:12">
       <c r="A322">
         <v>19860718</v>
       </c>
@@ -13499,7 +13735,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="323" spans="1:8">
+    <row r="323" spans="1:12">
       <c r="A323">
         <v>19860721</v>
       </c>
@@ -13510,7 +13746,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="324" spans="1:8">
+    <row r="324" spans="1:12">
       <c r="A324">
         <v>19860722</v>
       </c>
@@ -13521,7 +13757,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="325" spans="1:8">
+    <row r="325" spans="1:12">
       <c r="A325">
         <v>19860724</v>
       </c>
@@ -13532,7 +13768,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="326" spans="1:8">
+    <row r="326" spans="1:12">
       <c r="A326">
         <v>19860728</v>
       </c>
@@ -13543,7 +13779,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:12">
       <c r="A327">
         <v>19860729</v>
       </c>
@@ -13554,7 +13790,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="328" spans="1:8">
+    <row r="328" spans="1:12">
       <c r="A328">
         <v>19860730</v>
       </c>
@@ -13565,7 +13801,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="329" spans="1:8">
+    <row r="329" spans="1:12">
       <c r="A329">
         <v>19860731</v>
       </c>
@@ -13576,7 +13812,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="330" spans="1:8">
+    <row r="330" spans="1:12">
       <c r="A330">
         <v>19860804</v>
       </c>
@@ -13587,7 +13823,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="331" spans="1:8">
+    <row r="331" spans="1:12">
       <c r="A331">
         <v>19860805</v>
       </c>
@@ -13598,7 +13834,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="332" spans="1:8">
+    <row r="332" spans="1:12">
       <c r="A332">
         <v>19860806</v>
       </c>
@@ -13624,8 +13860,20 @@
         <f>AVERAGE(C314:C332)</f>
         <v>660.52631578947364</v>
       </c>
-    </row>
-    <row r="333" spans="1:8">
+      <c r="I332" t="s">
+        <v>7</v>
+      </c>
+      <c r="J332" t="s">
+        <v>7</v>
+      </c>
+      <c r="K332" t="s">
+        <v>7</v>
+      </c>
+      <c r="L332" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" spans="1:12">
       <c r="A333">
         <v>19860808</v>
       </c>
@@ -13636,7 +13884,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:12">
       <c r="A334">
         <v>19860811</v>
       </c>
@@ -13647,7 +13895,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:12">
       <c r="A335">
         <v>19860812</v>
       </c>
@@ -13658,7 +13906,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="336" spans="1:8">
+    <row r="336" spans="1:12">
       <c r="A336">
         <v>19860813</v>
       </c>
@@ -13669,7 +13917,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="337" spans="1:8">
+    <row r="337" spans="1:12">
       <c r="A337">
         <v>19860814</v>
       </c>
@@ -13680,7 +13928,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="338" spans="1:8">
+    <row r="338" spans="1:12">
       <c r="A338">
         <v>19860815</v>
       </c>
@@ -13691,7 +13939,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="339" spans="1:8">
+    <row r="339" spans="1:12">
       <c r="A339">
         <v>19860818</v>
       </c>
@@ -13702,7 +13950,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="340" spans="1:8">
+    <row r="340" spans="1:12">
       <c r="A340">
         <v>19860819</v>
       </c>
@@ -13713,7 +13961,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="341" spans="1:8">
+    <row r="341" spans="1:12">
       <c r="A341">
         <v>19860820</v>
       </c>
@@ -13724,7 +13972,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="342" spans="1:8">
+    <row r="342" spans="1:12">
       <c r="A342">
         <v>19860821</v>
       </c>
@@ -13746,8 +13994,24 @@
       <c r="H342" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="343" spans="1:8">
+      <c r="I342">
+        <f>SUM(B342:B359)</f>
+        <v>780</v>
+      </c>
+      <c r="J342">
+        <f>SUM(C342:C359)</f>
+        <v>18400</v>
+      </c>
+      <c r="K342">
+        <f>AVERAGE(B342:B359)</f>
+        <v>43.333333333333336</v>
+      </c>
+      <c r="L342">
+        <f>AVERAGE(C342:C359)</f>
+        <v>1022.2222222222222</v>
+      </c>
+    </row>
+    <row r="343" spans="1:12">
       <c r="A343">
         <v>19860822</v>
       </c>
@@ -13758,7 +14022,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="344" spans="1:8">
+    <row r="344" spans="1:12">
       <c r="A344">
         <v>19860825</v>
       </c>
@@ -13769,7 +14033,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="345" spans="1:8">
+    <row r="345" spans="1:12">
       <c r="A345">
         <v>19860826</v>
       </c>
@@ -13780,7 +14044,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="346" spans="1:8">
+    <row r="346" spans="1:12">
       <c r="A346">
         <v>19860827</v>
       </c>
@@ -13791,7 +14055,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:12">
       <c r="A347">
         <v>19860828</v>
       </c>
@@ -13802,7 +14066,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="348" spans="1:8">
+    <row r="348" spans="1:12">
       <c r="A348">
         <v>19860829</v>
       </c>
@@ -13813,7 +14077,7 @@
         <v>5850</v>
       </c>
     </row>
-    <row r="349" spans="1:8">
+    <row r="349" spans="1:12">
       <c r="A349">
         <v>19860902</v>
       </c>
@@ -13824,7 +14088,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="350" spans="1:8">
+    <row r="350" spans="1:12">
       <c r="A350">
         <v>19860903</v>
       </c>
@@ -13835,7 +14099,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="351" spans="1:8">
+    <row r="351" spans="1:12">
       <c r="A351">
         <v>19860904</v>
       </c>
@@ -13846,7 +14110,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="352" spans="1:8">
+    <row r="352" spans="1:12">
       <c r="A352">
         <v>19860905</v>
       </c>
@@ -13857,7 +14121,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="353" spans="1:8">
+    <row r="353" spans="1:12">
       <c r="A353">
         <v>19860908</v>
       </c>
@@ -13868,7 +14132,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="354" spans="1:8">
+    <row r="354" spans="1:12">
       <c r="A354">
         <v>19860909</v>
       </c>
@@ -13879,7 +14143,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="355" spans="1:8">
+    <row r="355" spans="1:12">
       <c r="A355">
         <v>19860911</v>
       </c>
@@ -13890,7 +14154,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="356" spans="1:8">
+    <row r="356" spans="1:12">
       <c r="A356">
         <v>19860912</v>
       </c>
@@ -13901,7 +14165,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="357" spans="1:8">
+    <row r="357" spans="1:12">
       <c r="A357">
         <v>19860915</v>
       </c>
@@ -13912,7 +14176,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="358" spans="1:8">
+    <row r="358" spans="1:12">
       <c r="A358">
         <v>19860918</v>
       </c>
@@ -13923,7 +14187,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="359" spans="1:8">
+    <row r="359" spans="1:12">
       <c r="A359">
         <v>19860923</v>
       </c>
@@ -13949,8 +14213,20 @@
         <f>AVERAGE(C342:C359)</f>
         <v>1022.2222222222222</v>
       </c>
-    </row>
-    <row r="360" spans="1:8">
+      <c r="I359" t="s">
+        <v>7</v>
+      </c>
+      <c r="J359" t="s">
+        <v>7</v>
+      </c>
+      <c r="K359" t="s">
+        <v>7</v>
+      </c>
+      <c r="L359" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="360" spans="1:12">
       <c r="A360">
         <v>19860925</v>
       </c>
@@ -13961,7 +14237,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="361" spans="1:8">
+    <row r="361" spans="1:12">
       <c r="A361">
         <v>19860926</v>
       </c>
@@ -13972,7 +14248,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="362" spans="1:8">
+    <row r="362" spans="1:12">
       <c r="A362">
         <v>19860929</v>
       </c>
@@ -13983,7 +14259,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="363" spans="1:8">
+    <row r="363" spans="1:12">
       <c r="A363">
         <v>19861002</v>
       </c>
@@ -13994,7 +14270,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="364" spans="1:8">
+    <row r="364" spans="1:12">
       <c r="A364">
         <v>19861003</v>
       </c>
@@ -14005,7 +14281,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="365" spans="1:8">
+    <row r="365" spans="1:12">
       <c r="A365">
         <v>19861007</v>
       </c>
@@ -14016,7 +14292,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="366" spans="1:8">
+    <row r="366" spans="1:12">
       <c r="A366">
         <v>19861013</v>
       </c>
@@ -14027,7 +14303,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="367" spans="1:8">
+    <row r="367" spans="1:12">
       <c r="A367">
         <v>19861014</v>
       </c>
@@ -14038,7 +14314,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="368" spans="1:8">
+    <row r="368" spans="1:12">
       <c r="A368">
         <v>19861015</v>
       </c>
@@ -63595,7 +63871,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="4865" spans="1:8">
+    <row r="4865" spans="1:12">
       <c r="A4865">
         <v>20160624</v>
       </c>
@@ -63606,7 +63882,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4866" spans="1:8">
+    <row r="4866" spans="1:12">
       <c r="A4866">
         <v>20160627</v>
       </c>
@@ -63617,7 +63893,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4867" spans="1:8">
+    <row r="4867" spans="1:12">
       <c r="A4867">
         <v>20160629</v>
       </c>
@@ -63628,7 +63904,7 @@
         <v>4966</v>
       </c>
     </row>
-    <row r="4868" spans="1:8">
+    <row r="4868" spans="1:12">
       <c r="A4868">
         <v>20160630</v>
       </c>
@@ -63639,7 +63915,7 @@
         <v>8072</v>
       </c>
     </row>
-    <row r="4869" spans="1:8">
+    <row r="4869" spans="1:12">
       <c r="A4869">
         <v>20160701</v>
       </c>
@@ -63650,7 +63926,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="4870" spans="1:8">
+    <row r="4870" spans="1:12">
       <c r="A4870">
         <v>20160705</v>
       </c>
@@ -63661,7 +63937,7 @@
         <v>8139</v>
       </c>
     </row>
-    <row r="4871" spans="1:8">
+    <row r="4871" spans="1:12">
       <c r="A4871">
         <v>20160707</v>
       </c>
@@ -63672,7 +63948,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4872" spans="1:8">
+    <row r="4872" spans="1:12">
       <c r="A4872">
         <v>20160708</v>
       </c>
@@ -63694,8 +63970,24 @@
       <c r="H4872" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4873" spans="1:8">
+      <c r="I4872">
+        <f>SUM(B4872:B4880)</f>
+        <v>800.17820000000006</v>
+      </c>
+      <c r="J4872">
+        <f>SUM(C4872:C4880)</f>
+        <v>23267</v>
+      </c>
+      <c r="K4872">
+        <f>AVERAGE(B4872:B4880)</f>
+        <v>88.908688888888889</v>
+      </c>
+      <c r="L4872">
+        <f>AVERAGE(C4872:C4880)</f>
+        <v>2585.2222222222222</v>
+      </c>
+    </row>
+    <row r="4873" spans="1:12">
       <c r="A4873">
         <v>20160711</v>
       </c>
@@ -63706,7 +63998,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="4874" spans="1:8">
+    <row r="4874" spans="1:12">
       <c r="A4874">
         <v>20160713</v>
       </c>
@@ -63717,7 +64009,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="4875" spans="1:8">
+    <row r="4875" spans="1:12">
       <c r="A4875">
         <v>20160715</v>
       </c>
@@ -63728,7 +64020,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4876" spans="1:8">
+    <row r="4876" spans="1:12">
       <c r="A4876">
         <v>20160718</v>
       </c>
@@ -63739,7 +64031,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="4877" spans="1:8">
+    <row r="4877" spans="1:12">
       <c r="A4877">
         <v>20160719</v>
       </c>
@@ -63750,7 +64042,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4878" spans="1:8">
+    <row r="4878" spans="1:12">
       <c r="A4878">
         <v>20160720</v>
       </c>
@@ -63761,7 +64053,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="4879" spans="1:8">
+    <row r="4879" spans="1:12">
       <c r="A4879">
         <v>20160721</v>
       </c>
@@ -63772,7 +64064,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="4880" spans="1:8">
+    <row r="4880" spans="1:12">
       <c r="A4880">
         <v>20160722</v>
       </c>
@@ -63797,6 +64089,18 @@
       <c r="H4880">
         <f>AVERAGE(C4872:C4880)</f>
         <v>2585.2222222222222</v>
+      </c>
+      <c r="I4880" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4880" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4880" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4880" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>